<commit_message>
testing until 70% line, 63% method, 60% class
</commit_message>
<xml_diff>
--- a/resources/map.xlsx
+++ b/resources/map.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nicol\Documents\GitHub\StoreGame\src\res\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nicol\Documents\GitHub\StoreGame\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6781BA85-86D5-4EF0-84DF-AA7F4A38D7F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B2EE30A-1EDC-43B4-8966-7F2029D1BE65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28800" yWindow="5445" windowWidth="28800" windowHeight="15885" xr2:uid="{56ED3418-DE84-4A29-B959-FE4D25080271}"/>
+    <workbookView xWindow="4770" yWindow="3210" windowWidth="28800" windowHeight="15885" xr2:uid="{56ED3418-DE84-4A29-B959-FE4D25080271}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="323" uniqueCount="6">
   <si>
     <t>WALL</t>
   </si>
@@ -44,10 +44,16 @@
     <t>GROUND</t>
   </si>
   <si>
-    <t>SHELF_N</t>
+    <t>SHELF_N_CC:aa</t>
   </si>
   <si>
-    <t>SHELF_S</t>
+    <t>SHELF_N_CC:ab</t>
+  </si>
+  <si>
+    <t>SHELF_S_CC:ac</t>
+  </si>
+  <si>
+    <t>SHELF_S_CC:ad</t>
   </si>
 </sst>
 </file>
@@ -419,15 +425,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{892ABF15-6683-43AF-9DBE-19CFF00B5E93}">
-  <dimension ref="A1:K27"/>
+  <dimension ref="A1:L27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+      <selection activeCell="M8" sqref="M8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -462,7 +468,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -496,8 +502,11 @@
       <c r="K2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -531,8 +540,11 @@
       <c r="K3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -552,22 +564,25 @@
         <v>2</v>
       </c>
       <c r="G4" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H4" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I4" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J4" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="K4" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>0</v>
       </c>
@@ -575,34 +590,37 @@
         <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D5" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E5" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F5" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G5" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="H5" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="I5" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="J5" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="K5" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>0</v>
       </c>
@@ -636,8 +654,11 @@
       <c r="K6" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>0</v>
       </c>
@@ -671,8 +692,11 @@
       <c r="K7" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L7" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>0</v>
       </c>
@@ -706,8 +730,11 @@
       <c r="K8" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L8" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>0</v>
       </c>
@@ -741,8 +768,11 @@
       <c r="K9" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L9" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>0</v>
       </c>
@@ -776,8 +806,11 @@
       <c r="K10" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L10" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>0</v>
       </c>
@@ -811,8 +844,11 @@
       <c r="K11" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L11" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>0</v>
       </c>
@@ -846,8 +882,11 @@
       <c r="K12" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L12" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>0</v>
       </c>
@@ -881,8 +920,11 @@
       <c r="K13" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L13" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>0</v>
       </c>
@@ -916,8 +958,11 @@
       <c r="K14" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L14" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>0</v>
       </c>
@@ -951,8 +996,11 @@
       <c r="K15" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L15" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>0</v>
       </c>
@@ -986,8 +1034,11 @@
       <c r="K16" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L16" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>0</v>
       </c>
@@ -1021,8 +1072,11 @@
       <c r="K17" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L17" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>0</v>
       </c>
@@ -1056,8 +1110,11 @@
       <c r="K18" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L18" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>0</v>
       </c>
@@ -1091,8 +1148,11 @@
       <c r="K19" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L19" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>0</v>
       </c>
@@ -1126,8 +1186,11 @@
       <c r="K20" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L20" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>0</v>
       </c>
@@ -1161,8 +1224,11 @@
       <c r="K21" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L21" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>0</v>
       </c>
@@ -1196,8 +1262,11 @@
       <c r="K22" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L22" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>0</v>
       </c>
@@ -1231,8 +1300,11 @@
       <c r="K23" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L23" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>0</v>
       </c>
@@ -1266,8 +1338,11 @@
       <c r="K24" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L24" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>0</v>
       </c>
@@ -1301,8 +1376,11 @@
       <c r="K25" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L25" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>0</v>
       </c>
@@ -1336,8 +1414,11 @@
       <c r="K26" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L26" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>0</v>
       </c>
@@ -1369,6 +1450,9 @@
         <v>1</v>
       </c>
       <c r="K27" t="s">
+        <v>1</v>
+      </c>
+      <c r="L27" t="s">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
IRender , RenderStrategy , camera stabilisation
Camera stabilisatie werkt nog niet helemaal. Als we per 1 verschuiven werkt het oke... Vanaf 2 verschuift hij soms door een verkeerde berekening
</commit_message>
<xml_diff>
--- a/resources/map.xlsx
+++ b/resources/map.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nicol\Documents\GitHub\StoreGame\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B2EE30A-1EDC-43B4-8966-7F2029D1BE65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD5E83DB-C24A-4101-A3AD-69DAAF11F1B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4770" yWindow="3210" windowWidth="28800" windowHeight="15885" xr2:uid="{56ED3418-DE84-4A29-B959-FE4D25080271}"/>
+    <workbookView xWindow="5115" yWindow="3555" windowWidth="28800" windowHeight="15885" xr2:uid="{56ED3418-DE84-4A29-B959-FE4D25080271}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="323" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="861" uniqueCount="6">
   <si>
     <t>WALL</t>
   </si>
@@ -425,15 +425,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{892ABF15-6683-43AF-9DBE-19CFF00B5E93}">
-  <dimension ref="A1:L27"/>
+  <dimension ref="A1:AG37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M8" sqref="M8"/>
+      <selection activeCell="L18" sqref="L18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -467,8 +467,74 @@
       <c r="K1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L1" t="s">
+        <v>0</v>
+      </c>
+      <c r="M1" t="s">
+        <v>0</v>
+      </c>
+      <c r="N1" t="s">
+        <v>0</v>
+      </c>
+      <c r="O1" t="s">
+        <v>0</v>
+      </c>
+      <c r="P1" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>0</v>
+      </c>
+      <c r="R1" t="s">
+        <v>0</v>
+      </c>
+      <c r="S1" t="s">
+        <v>0</v>
+      </c>
+      <c r="T1" t="s">
+        <v>0</v>
+      </c>
+      <c r="U1" t="s">
+        <v>0</v>
+      </c>
+      <c r="V1" t="s">
+        <v>0</v>
+      </c>
+      <c r="W1" t="s">
+        <v>0</v>
+      </c>
+      <c r="X1" t="s">
+        <v>0</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>0</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>0</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -505,8 +571,41 @@
       <c r="L2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M2" t="s">
+        <v>1</v>
+      </c>
+      <c r="N2" t="s">
+        <v>1</v>
+      </c>
+      <c r="O2" t="s">
+        <v>1</v>
+      </c>
+      <c r="P2" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>1</v>
+      </c>
+      <c r="R2" t="s">
+        <v>1</v>
+      </c>
+      <c r="S2" t="s">
+        <v>1</v>
+      </c>
+      <c r="T2" t="s">
+        <v>1</v>
+      </c>
+      <c r="U2" t="s">
+        <v>1</v>
+      </c>
+      <c r="V2" t="s">
+        <v>1</v>
+      </c>
+      <c r="W2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -543,8 +642,41 @@
       <c r="L3" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M3" t="s">
+        <v>1</v>
+      </c>
+      <c r="N3" t="s">
+        <v>1</v>
+      </c>
+      <c r="O3" t="s">
+        <v>1</v>
+      </c>
+      <c r="P3" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>1</v>
+      </c>
+      <c r="R3" t="s">
+        <v>1</v>
+      </c>
+      <c r="S3" t="s">
+        <v>1</v>
+      </c>
+      <c r="T3" t="s">
+        <v>1</v>
+      </c>
+      <c r="U3" t="s">
+        <v>1</v>
+      </c>
+      <c r="V3" t="s">
+        <v>1</v>
+      </c>
+      <c r="W3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -581,8 +713,41 @@
       <c r="L4" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M4" t="s">
+        <v>1</v>
+      </c>
+      <c r="N4" t="s">
+        <v>1</v>
+      </c>
+      <c r="O4" t="s">
+        <v>1</v>
+      </c>
+      <c r="P4" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>1</v>
+      </c>
+      <c r="R4" t="s">
+        <v>1</v>
+      </c>
+      <c r="S4" t="s">
+        <v>1</v>
+      </c>
+      <c r="T4" t="s">
+        <v>1</v>
+      </c>
+      <c r="U4" t="s">
+        <v>1</v>
+      </c>
+      <c r="V4" t="s">
+        <v>1</v>
+      </c>
+      <c r="W4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>0</v>
       </c>
@@ -619,8 +784,41 @@
       <c r="L5" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M5" t="s">
+        <v>1</v>
+      </c>
+      <c r="N5" t="s">
+        <v>1</v>
+      </c>
+      <c r="O5" t="s">
+        <v>1</v>
+      </c>
+      <c r="P5" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>1</v>
+      </c>
+      <c r="R5" t="s">
+        <v>1</v>
+      </c>
+      <c r="S5" t="s">
+        <v>1</v>
+      </c>
+      <c r="T5" t="s">
+        <v>1</v>
+      </c>
+      <c r="U5" t="s">
+        <v>1</v>
+      </c>
+      <c r="V5" t="s">
+        <v>1</v>
+      </c>
+      <c r="W5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>0</v>
       </c>
@@ -657,8 +855,41 @@
       <c r="L6" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M6" t="s">
+        <v>1</v>
+      </c>
+      <c r="N6" t="s">
+        <v>1</v>
+      </c>
+      <c r="O6" t="s">
+        <v>1</v>
+      </c>
+      <c r="P6" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>1</v>
+      </c>
+      <c r="R6" t="s">
+        <v>1</v>
+      </c>
+      <c r="S6" t="s">
+        <v>1</v>
+      </c>
+      <c r="T6" t="s">
+        <v>1</v>
+      </c>
+      <c r="U6" t="s">
+        <v>1</v>
+      </c>
+      <c r="V6" t="s">
+        <v>1</v>
+      </c>
+      <c r="W6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>0</v>
       </c>
@@ -695,8 +926,41 @@
       <c r="L7" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M7" t="s">
+        <v>1</v>
+      </c>
+      <c r="N7" t="s">
+        <v>1</v>
+      </c>
+      <c r="O7" t="s">
+        <v>1</v>
+      </c>
+      <c r="P7" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>1</v>
+      </c>
+      <c r="R7" t="s">
+        <v>1</v>
+      </c>
+      <c r="S7" t="s">
+        <v>1</v>
+      </c>
+      <c r="T7" t="s">
+        <v>1</v>
+      </c>
+      <c r="U7" t="s">
+        <v>1</v>
+      </c>
+      <c r="V7" t="s">
+        <v>1</v>
+      </c>
+      <c r="W7" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>0</v>
       </c>
@@ -733,8 +997,41 @@
       <c r="L8" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M8" t="s">
+        <v>1</v>
+      </c>
+      <c r="N8" t="s">
+        <v>1</v>
+      </c>
+      <c r="O8" t="s">
+        <v>1</v>
+      </c>
+      <c r="P8" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>1</v>
+      </c>
+      <c r="R8" t="s">
+        <v>1</v>
+      </c>
+      <c r="S8" t="s">
+        <v>1</v>
+      </c>
+      <c r="T8" t="s">
+        <v>1</v>
+      </c>
+      <c r="U8" t="s">
+        <v>1</v>
+      </c>
+      <c r="V8" t="s">
+        <v>1</v>
+      </c>
+      <c r="W8" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>0</v>
       </c>
@@ -771,8 +1068,41 @@
       <c r="L9" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M9" t="s">
+        <v>1</v>
+      </c>
+      <c r="N9" t="s">
+        <v>1</v>
+      </c>
+      <c r="O9" t="s">
+        <v>1</v>
+      </c>
+      <c r="P9" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>1</v>
+      </c>
+      <c r="R9" t="s">
+        <v>1</v>
+      </c>
+      <c r="S9" t="s">
+        <v>1</v>
+      </c>
+      <c r="T9" t="s">
+        <v>1</v>
+      </c>
+      <c r="U9" t="s">
+        <v>1</v>
+      </c>
+      <c r="V9" t="s">
+        <v>1</v>
+      </c>
+      <c r="W9" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>0</v>
       </c>
@@ -809,8 +1139,41 @@
       <c r="L10" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M10" t="s">
+        <v>1</v>
+      </c>
+      <c r="N10" t="s">
+        <v>1</v>
+      </c>
+      <c r="O10" t="s">
+        <v>1</v>
+      </c>
+      <c r="P10" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>1</v>
+      </c>
+      <c r="R10" t="s">
+        <v>1</v>
+      </c>
+      <c r="S10" t="s">
+        <v>1</v>
+      </c>
+      <c r="T10" t="s">
+        <v>1</v>
+      </c>
+      <c r="U10" t="s">
+        <v>1</v>
+      </c>
+      <c r="V10" t="s">
+        <v>1</v>
+      </c>
+      <c r="W10" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>0</v>
       </c>
@@ -847,8 +1210,41 @@
       <c r="L11" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M11" t="s">
+        <v>1</v>
+      </c>
+      <c r="N11" t="s">
+        <v>1</v>
+      </c>
+      <c r="O11" t="s">
+        <v>1</v>
+      </c>
+      <c r="P11" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>1</v>
+      </c>
+      <c r="R11" t="s">
+        <v>1</v>
+      </c>
+      <c r="S11" t="s">
+        <v>1</v>
+      </c>
+      <c r="T11" t="s">
+        <v>1</v>
+      </c>
+      <c r="U11" t="s">
+        <v>1</v>
+      </c>
+      <c r="V11" t="s">
+        <v>1</v>
+      </c>
+      <c r="W11" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>0</v>
       </c>
@@ -885,8 +1281,41 @@
       <c r="L12" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M12" t="s">
+        <v>1</v>
+      </c>
+      <c r="N12" t="s">
+        <v>1</v>
+      </c>
+      <c r="O12" t="s">
+        <v>1</v>
+      </c>
+      <c r="P12" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q12" t="s">
+        <v>1</v>
+      </c>
+      <c r="R12" t="s">
+        <v>1</v>
+      </c>
+      <c r="S12" t="s">
+        <v>1</v>
+      </c>
+      <c r="T12" t="s">
+        <v>1</v>
+      </c>
+      <c r="U12" t="s">
+        <v>1</v>
+      </c>
+      <c r="V12" t="s">
+        <v>1</v>
+      </c>
+      <c r="W12" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>0</v>
       </c>
@@ -923,8 +1352,41 @@
       <c r="L13" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M13" t="s">
+        <v>1</v>
+      </c>
+      <c r="N13" t="s">
+        <v>1</v>
+      </c>
+      <c r="O13" t="s">
+        <v>1</v>
+      </c>
+      <c r="P13" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q13" t="s">
+        <v>1</v>
+      </c>
+      <c r="R13" t="s">
+        <v>1</v>
+      </c>
+      <c r="S13" t="s">
+        <v>1</v>
+      </c>
+      <c r="T13" t="s">
+        <v>1</v>
+      </c>
+      <c r="U13" t="s">
+        <v>1</v>
+      </c>
+      <c r="V13" t="s">
+        <v>1</v>
+      </c>
+      <c r="W13" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>0</v>
       </c>
@@ -961,8 +1423,41 @@
       <c r="L14" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M14" t="s">
+        <v>1</v>
+      </c>
+      <c r="N14" t="s">
+        <v>1</v>
+      </c>
+      <c r="O14" t="s">
+        <v>1</v>
+      </c>
+      <c r="P14" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q14" t="s">
+        <v>1</v>
+      </c>
+      <c r="R14" t="s">
+        <v>1</v>
+      </c>
+      <c r="S14" t="s">
+        <v>1</v>
+      </c>
+      <c r="T14" t="s">
+        <v>1</v>
+      </c>
+      <c r="U14" t="s">
+        <v>1</v>
+      </c>
+      <c r="V14" t="s">
+        <v>1</v>
+      </c>
+      <c r="W14" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>0</v>
       </c>
@@ -999,8 +1494,41 @@
       <c r="L15" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M15" t="s">
+        <v>1</v>
+      </c>
+      <c r="N15" t="s">
+        <v>1</v>
+      </c>
+      <c r="O15" t="s">
+        <v>1</v>
+      </c>
+      <c r="P15" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q15" t="s">
+        <v>1</v>
+      </c>
+      <c r="R15" t="s">
+        <v>1</v>
+      </c>
+      <c r="S15" t="s">
+        <v>1</v>
+      </c>
+      <c r="T15" t="s">
+        <v>1</v>
+      </c>
+      <c r="U15" t="s">
+        <v>1</v>
+      </c>
+      <c r="V15" t="s">
+        <v>1</v>
+      </c>
+      <c r="W15" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>0</v>
       </c>
@@ -1037,8 +1565,41 @@
       <c r="L16" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M16" t="s">
+        <v>1</v>
+      </c>
+      <c r="N16" t="s">
+        <v>1</v>
+      </c>
+      <c r="O16" t="s">
+        <v>1</v>
+      </c>
+      <c r="P16" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q16" t="s">
+        <v>1</v>
+      </c>
+      <c r="R16" t="s">
+        <v>1</v>
+      </c>
+      <c r="S16" t="s">
+        <v>1</v>
+      </c>
+      <c r="T16" t="s">
+        <v>1</v>
+      </c>
+      <c r="U16" t="s">
+        <v>1</v>
+      </c>
+      <c r="V16" t="s">
+        <v>1</v>
+      </c>
+      <c r="W16" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>0</v>
       </c>
@@ -1075,8 +1636,41 @@
       <c r="L17" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M17" t="s">
+        <v>1</v>
+      </c>
+      <c r="N17" t="s">
+        <v>1</v>
+      </c>
+      <c r="O17" t="s">
+        <v>1</v>
+      </c>
+      <c r="P17" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q17" t="s">
+        <v>1</v>
+      </c>
+      <c r="R17" t="s">
+        <v>1</v>
+      </c>
+      <c r="S17" t="s">
+        <v>1</v>
+      </c>
+      <c r="T17" t="s">
+        <v>1</v>
+      </c>
+      <c r="U17" t="s">
+        <v>1</v>
+      </c>
+      <c r="V17" t="s">
+        <v>1</v>
+      </c>
+      <c r="W17" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>0</v>
       </c>
@@ -1113,8 +1707,41 @@
       <c r="L18" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M18" t="s">
+        <v>1</v>
+      </c>
+      <c r="N18" t="s">
+        <v>1</v>
+      </c>
+      <c r="O18" t="s">
+        <v>1</v>
+      </c>
+      <c r="P18" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q18" t="s">
+        <v>1</v>
+      </c>
+      <c r="R18" t="s">
+        <v>1</v>
+      </c>
+      <c r="S18" t="s">
+        <v>1</v>
+      </c>
+      <c r="T18" t="s">
+        <v>1</v>
+      </c>
+      <c r="U18" t="s">
+        <v>1</v>
+      </c>
+      <c r="V18" t="s">
+        <v>1</v>
+      </c>
+      <c r="W18" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>0</v>
       </c>
@@ -1151,8 +1778,41 @@
       <c r="L19" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M19" t="s">
+        <v>1</v>
+      </c>
+      <c r="N19" t="s">
+        <v>1</v>
+      </c>
+      <c r="O19" t="s">
+        <v>1</v>
+      </c>
+      <c r="P19" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q19" t="s">
+        <v>1</v>
+      </c>
+      <c r="R19" t="s">
+        <v>1</v>
+      </c>
+      <c r="S19" t="s">
+        <v>1</v>
+      </c>
+      <c r="T19" t="s">
+        <v>1</v>
+      </c>
+      <c r="U19" t="s">
+        <v>1</v>
+      </c>
+      <c r="V19" t="s">
+        <v>1</v>
+      </c>
+      <c r="W19" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>0</v>
       </c>
@@ -1189,8 +1849,41 @@
       <c r="L20" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M20" t="s">
+        <v>1</v>
+      </c>
+      <c r="N20" t="s">
+        <v>1</v>
+      </c>
+      <c r="O20" t="s">
+        <v>1</v>
+      </c>
+      <c r="P20" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q20" t="s">
+        <v>1</v>
+      </c>
+      <c r="R20" t="s">
+        <v>1</v>
+      </c>
+      <c r="S20" t="s">
+        <v>1</v>
+      </c>
+      <c r="T20" t="s">
+        <v>1</v>
+      </c>
+      <c r="U20" t="s">
+        <v>1</v>
+      </c>
+      <c r="V20" t="s">
+        <v>1</v>
+      </c>
+      <c r="W20" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>0</v>
       </c>
@@ -1227,8 +1920,41 @@
       <c r="L21" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M21" t="s">
+        <v>1</v>
+      </c>
+      <c r="N21" t="s">
+        <v>1</v>
+      </c>
+      <c r="O21" t="s">
+        <v>1</v>
+      </c>
+      <c r="P21" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q21" t="s">
+        <v>1</v>
+      </c>
+      <c r="R21" t="s">
+        <v>1</v>
+      </c>
+      <c r="S21" t="s">
+        <v>1</v>
+      </c>
+      <c r="T21" t="s">
+        <v>1</v>
+      </c>
+      <c r="U21" t="s">
+        <v>1</v>
+      </c>
+      <c r="V21" t="s">
+        <v>1</v>
+      </c>
+      <c r="W21" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>0</v>
       </c>
@@ -1265,8 +1991,41 @@
       <c r="L22" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M22" t="s">
+        <v>1</v>
+      </c>
+      <c r="N22" t="s">
+        <v>1</v>
+      </c>
+      <c r="O22" t="s">
+        <v>1</v>
+      </c>
+      <c r="P22" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q22" t="s">
+        <v>1</v>
+      </c>
+      <c r="R22" t="s">
+        <v>1</v>
+      </c>
+      <c r="S22" t="s">
+        <v>1</v>
+      </c>
+      <c r="T22" t="s">
+        <v>1</v>
+      </c>
+      <c r="U22" t="s">
+        <v>1</v>
+      </c>
+      <c r="V22" t="s">
+        <v>1</v>
+      </c>
+      <c r="W22" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>0</v>
       </c>
@@ -1303,8 +2062,41 @@
       <c r="L23" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M23" t="s">
+        <v>1</v>
+      </c>
+      <c r="N23" t="s">
+        <v>1</v>
+      </c>
+      <c r="O23" t="s">
+        <v>1</v>
+      </c>
+      <c r="P23" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q23" t="s">
+        <v>1</v>
+      </c>
+      <c r="R23" t="s">
+        <v>1</v>
+      </c>
+      <c r="S23" t="s">
+        <v>1</v>
+      </c>
+      <c r="T23" t="s">
+        <v>1</v>
+      </c>
+      <c r="U23" t="s">
+        <v>1</v>
+      </c>
+      <c r="V23" t="s">
+        <v>1</v>
+      </c>
+      <c r="W23" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>0</v>
       </c>
@@ -1341,8 +2133,41 @@
       <c r="L24" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M24" t="s">
+        <v>1</v>
+      </c>
+      <c r="N24" t="s">
+        <v>1</v>
+      </c>
+      <c r="O24" t="s">
+        <v>1</v>
+      </c>
+      <c r="P24" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q24" t="s">
+        <v>1</v>
+      </c>
+      <c r="R24" t="s">
+        <v>1</v>
+      </c>
+      <c r="S24" t="s">
+        <v>1</v>
+      </c>
+      <c r="T24" t="s">
+        <v>1</v>
+      </c>
+      <c r="U24" t="s">
+        <v>1</v>
+      </c>
+      <c r="V24" t="s">
+        <v>1</v>
+      </c>
+      <c r="W24" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>0</v>
       </c>
@@ -1379,8 +2204,41 @@
       <c r="L25" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M25" t="s">
+        <v>1</v>
+      </c>
+      <c r="N25" t="s">
+        <v>1</v>
+      </c>
+      <c r="O25" t="s">
+        <v>1</v>
+      </c>
+      <c r="P25" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q25" t="s">
+        <v>1</v>
+      </c>
+      <c r="R25" t="s">
+        <v>1</v>
+      </c>
+      <c r="S25" t="s">
+        <v>1</v>
+      </c>
+      <c r="T25" t="s">
+        <v>1</v>
+      </c>
+      <c r="U25" t="s">
+        <v>1</v>
+      </c>
+      <c r="V25" t="s">
+        <v>1</v>
+      </c>
+      <c r="W25" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>0</v>
       </c>
@@ -1417,8 +2275,41 @@
       <c r="L26" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M26" t="s">
+        <v>1</v>
+      </c>
+      <c r="N26" t="s">
+        <v>1</v>
+      </c>
+      <c r="O26" t="s">
+        <v>1</v>
+      </c>
+      <c r="P26" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q26" t="s">
+        <v>1</v>
+      </c>
+      <c r="R26" t="s">
+        <v>1</v>
+      </c>
+      <c r="S26" t="s">
+        <v>1</v>
+      </c>
+      <c r="T26" t="s">
+        <v>1</v>
+      </c>
+      <c r="U26" t="s">
+        <v>1</v>
+      </c>
+      <c r="V26" t="s">
+        <v>1</v>
+      </c>
+      <c r="W26" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>0</v>
       </c>
@@ -1453,6 +2344,749 @@
         <v>1</v>
       </c>
       <c r="L27" t="s">
+        <v>1</v>
+      </c>
+      <c r="M27" t="s">
+        <v>1</v>
+      </c>
+      <c r="N27" t="s">
+        <v>1</v>
+      </c>
+      <c r="O27" t="s">
+        <v>1</v>
+      </c>
+      <c r="P27" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q27" t="s">
+        <v>1</v>
+      </c>
+      <c r="R27" t="s">
+        <v>1</v>
+      </c>
+      <c r="S27" t="s">
+        <v>1</v>
+      </c>
+      <c r="T27" t="s">
+        <v>1</v>
+      </c>
+      <c r="U27" t="s">
+        <v>1</v>
+      </c>
+      <c r="V27" t="s">
+        <v>1</v>
+      </c>
+      <c r="W27" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>0</v>
+      </c>
+      <c r="B28" t="s">
+        <v>1</v>
+      </c>
+      <c r="C28" t="s">
+        <v>1</v>
+      </c>
+      <c r="D28" t="s">
+        <v>1</v>
+      </c>
+      <c r="E28" t="s">
+        <v>1</v>
+      </c>
+      <c r="F28" t="s">
+        <v>1</v>
+      </c>
+      <c r="G28" t="s">
+        <v>1</v>
+      </c>
+      <c r="H28" t="s">
+        <v>1</v>
+      </c>
+      <c r="I28" t="s">
+        <v>1</v>
+      </c>
+      <c r="J28" t="s">
+        <v>1</v>
+      </c>
+      <c r="K28" t="s">
+        <v>1</v>
+      </c>
+      <c r="L28" t="s">
+        <v>1</v>
+      </c>
+      <c r="M28" t="s">
+        <v>1</v>
+      </c>
+      <c r="N28" t="s">
+        <v>1</v>
+      </c>
+      <c r="O28" t="s">
+        <v>1</v>
+      </c>
+      <c r="P28" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q28" t="s">
+        <v>1</v>
+      </c>
+      <c r="R28" t="s">
+        <v>1</v>
+      </c>
+      <c r="S28" t="s">
+        <v>1</v>
+      </c>
+      <c r="T28" t="s">
+        <v>1</v>
+      </c>
+      <c r="U28" t="s">
+        <v>1</v>
+      </c>
+      <c r="V28" t="s">
+        <v>1</v>
+      </c>
+      <c r="W28" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>0</v>
+      </c>
+      <c r="B29" t="s">
+        <v>1</v>
+      </c>
+      <c r="C29" t="s">
+        <v>1</v>
+      </c>
+      <c r="D29" t="s">
+        <v>1</v>
+      </c>
+      <c r="E29" t="s">
+        <v>1</v>
+      </c>
+      <c r="F29" t="s">
+        <v>1</v>
+      </c>
+      <c r="G29" t="s">
+        <v>1</v>
+      </c>
+      <c r="H29" t="s">
+        <v>1</v>
+      </c>
+      <c r="I29" t="s">
+        <v>1</v>
+      </c>
+      <c r="J29" t="s">
+        <v>1</v>
+      </c>
+      <c r="K29" t="s">
+        <v>1</v>
+      </c>
+      <c r="L29" t="s">
+        <v>1</v>
+      </c>
+      <c r="M29" t="s">
+        <v>1</v>
+      </c>
+      <c r="N29" t="s">
+        <v>1</v>
+      </c>
+      <c r="O29" t="s">
+        <v>1</v>
+      </c>
+      <c r="P29" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q29" t="s">
+        <v>1</v>
+      </c>
+      <c r="R29" t="s">
+        <v>1</v>
+      </c>
+      <c r="S29" t="s">
+        <v>1</v>
+      </c>
+      <c r="T29" t="s">
+        <v>1</v>
+      </c>
+      <c r="U29" t="s">
+        <v>1</v>
+      </c>
+      <c r="V29" t="s">
+        <v>1</v>
+      </c>
+      <c r="W29" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>0</v>
+      </c>
+      <c r="B30" t="s">
+        <v>1</v>
+      </c>
+      <c r="C30" t="s">
+        <v>1</v>
+      </c>
+      <c r="D30" t="s">
+        <v>1</v>
+      </c>
+      <c r="E30" t="s">
+        <v>1</v>
+      </c>
+      <c r="F30" t="s">
+        <v>1</v>
+      </c>
+      <c r="G30" t="s">
+        <v>1</v>
+      </c>
+      <c r="H30" t="s">
+        <v>1</v>
+      </c>
+      <c r="I30" t="s">
+        <v>1</v>
+      </c>
+      <c r="J30" t="s">
+        <v>1</v>
+      </c>
+      <c r="K30" t="s">
+        <v>1</v>
+      </c>
+      <c r="L30" t="s">
+        <v>1</v>
+      </c>
+      <c r="M30" t="s">
+        <v>1</v>
+      </c>
+      <c r="N30" t="s">
+        <v>1</v>
+      </c>
+      <c r="O30" t="s">
+        <v>1</v>
+      </c>
+      <c r="P30" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q30" t="s">
+        <v>1</v>
+      </c>
+      <c r="R30" t="s">
+        <v>1</v>
+      </c>
+      <c r="S30" t="s">
+        <v>1</v>
+      </c>
+      <c r="T30" t="s">
+        <v>1</v>
+      </c>
+      <c r="U30" t="s">
+        <v>1</v>
+      </c>
+      <c r="V30" t="s">
+        <v>1</v>
+      </c>
+      <c r="W30" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>0</v>
+      </c>
+      <c r="B31" t="s">
+        <v>1</v>
+      </c>
+      <c r="C31" t="s">
+        <v>1</v>
+      </c>
+      <c r="D31" t="s">
+        <v>1</v>
+      </c>
+      <c r="E31" t="s">
+        <v>1</v>
+      </c>
+      <c r="F31" t="s">
+        <v>1</v>
+      </c>
+      <c r="G31" t="s">
+        <v>1</v>
+      </c>
+      <c r="H31" t="s">
+        <v>1</v>
+      </c>
+      <c r="I31" t="s">
+        <v>1</v>
+      </c>
+      <c r="J31" t="s">
+        <v>1</v>
+      </c>
+      <c r="K31" t="s">
+        <v>1</v>
+      </c>
+      <c r="L31" t="s">
+        <v>1</v>
+      </c>
+      <c r="M31" t="s">
+        <v>1</v>
+      </c>
+      <c r="N31" t="s">
+        <v>1</v>
+      </c>
+      <c r="O31" t="s">
+        <v>1</v>
+      </c>
+      <c r="P31" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q31" t="s">
+        <v>1</v>
+      </c>
+      <c r="R31" t="s">
+        <v>1</v>
+      </c>
+      <c r="S31" t="s">
+        <v>1</v>
+      </c>
+      <c r="T31" t="s">
+        <v>1</v>
+      </c>
+      <c r="U31" t="s">
+        <v>1</v>
+      </c>
+      <c r="V31" t="s">
+        <v>1</v>
+      </c>
+      <c r="W31" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>0</v>
+      </c>
+      <c r="B32" t="s">
+        <v>1</v>
+      </c>
+      <c r="C32" t="s">
+        <v>1</v>
+      </c>
+      <c r="D32" t="s">
+        <v>1</v>
+      </c>
+      <c r="E32" t="s">
+        <v>1</v>
+      </c>
+      <c r="F32" t="s">
+        <v>1</v>
+      </c>
+      <c r="G32" t="s">
+        <v>1</v>
+      </c>
+      <c r="H32" t="s">
+        <v>1</v>
+      </c>
+      <c r="I32" t="s">
+        <v>1</v>
+      </c>
+      <c r="J32" t="s">
+        <v>1</v>
+      </c>
+      <c r="K32" t="s">
+        <v>1</v>
+      </c>
+      <c r="L32" t="s">
+        <v>1</v>
+      </c>
+      <c r="M32" t="s">
+        <v>1</v>
+      </c>
+      <c r="N32" t="s">
+        <v>1</v>
+      </c>
+      <c r="O32" t="s">
+        <v>1</v>
+      </c>
+      <c r="P32" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q32" t="s">
+        <v>1</v>
+      </c>
+      <c r="R32" t="s">
+        <v>1</v>
+      </c>
+      <c r="S32" t="s">
+        <v>1</v>
+      </c>
+      <c r="T32" t="s">
+        <v>1</v>
+      </c>
+      <c r="U32" t="s">
+        <v>1</v>
+      </c>
+      <c r="V32" t="s">
+        <v>1</v>
+      </c>
+      <c r="W32" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>0</v>
+      </c>
+      <c r="B33" t="s">
+        <v>1</v>
+      </c>
+      <c r="C33" t="s">
+        <v>1</v>
+      </c>
+      <c r="D33" t="s">
+        <v>1</v>
+      </c>
+      <c r="E33" t="s">
+        <v>1</v>
+      </c>
+      <c r="F33" t="s">
+        <v>1</v>
+      </c>
+      <c r="G33" t="s">
+        <v>1</v>
+      </c>
+      <c r="H33" t="s">
+        <v>1</v>
+      </c>
+      <c r="I33" t="s">
+        <v>1</v>
+      </c>
+      <c r="J33" t="s">
+        <v>1</v>
+      </c>
+      <c r="K33" t="s">
+        <v>1</v>
+      </c>
+      <c r="L33" t="s">
+        <v>1</v>
+      </c>
+      <c r="M33" t="s">
+        <v>1</v>
+      </c>
+      <c r="N33" t="s">
+        <v>1</v>
+      </c>
+      <c r="O33" t="s">
+        <v>1</v>
+      </c>
+      <c r="P33" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q33" t="s">
+        <v>1</v>
+      </c>
+      <c r="R33" t="s">
+        <v>1</v>
+      </c>
+      <c r="S33" t="s">
+        <v>1</v>
+      </c>
+      <c r="T33" t="s">
+        <v>1</v>
+      </c>
+      <c r="U33" t="s">
+        <v>1</v>
+      </c>
+      <c r="V33" t="s">
+        <v>1</v>
+      </c>
+      <c r="W33" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>0</v>
+      </c>
+      <c r="B34" t="s">
+        <v>1</v>
+      </c>
+      <c r="C34" t="s">
+        <v>1</v>
+      </c>
+      <c r="D34" t="s">
+        <v>1</v>
+      </c>
+      <c r="E34" t="s">
+        <v>1</v>
+      </c>
+      <c r="F34" t="s">
+        <v>1</v>
+      </c>
+      <c r="G34" t="s">
+        <v>1</v>
+      </c>
+      <c r="H34" t="s">
+        <v>1</v>
+      </c>
+      <c r="I34" t="s">
+        <v>1</v>
+      </c>
+      <c r="J34" t="s">
+        <v>1</v>
+      </c>
+      <c r="K34" t="s">
+        <v>1</v>
+      </c>
+      <c r="L34" t="s">
+        <v>1</v>
+      </c>
+      <c r="M34" t="s">
+        <v>1</v>
+      </c>
+      <c r="N34" t="s">
+        <v>1</v>
+      </c>
+      <c r="O34" t="s">
+        <v>1</v>
+      </c>
+      <c r="P34" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q34" t="s">
+        <v>1</v>
+      </c>
+      <c r="R34" t="s">
+        <v>1</v>
+      </c>
+      <c r="S34" t="s">
+        <v>1</v>
+      </c>
+      <c r="T34" t="s">
+        <v>1</v>
+      </c>
+      <c r="U34" t="s">
+        <v>1</v>
+      </c>
+      <c r="V34" t="s">
+        <v>1</v>
+      </c>
+      <c r="W34" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>0</v>
+      </c>
+      <c r="B35" t="s">
+        <v>1</v>
+      </c>
+      <c r="C35" t="s">
+        <v>1</v>
+      </c>
+      <c r="D35" t="s">
+        <v>1</v>
+      </c>
+      <c r="E35" t="s">
+        <v>1</v>
+      </c>
+      <c r="F35" t="s">
+        <v>1</v>
+      </c>
+      <c r="G35" t="s">
+        <v>1</v>
+      </c>
+      <c r="H35" t="s">
+        <v>1</v>
+      </c>
+      <c r="I35" t="s">
+        <v>1</v>
+      </c>
+      <c r="J35" t="s">
+        <v>1</v>
+      </c>
+      <c r="K35" t="s">
+        <v>1</v>
+      </c>
+      <c r="L35" t="s">
+        <v>1</v>
+      </c>
+      <c r="M35" t="s">
+        <v>1</v>
+      </c>
+      <c r="N35" t="s">
+        <v>1</v>
+      </c>
+      <c r="O35" t="s">
+        <v>1</v>
+      </c>
+      <c r="P35" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q35" t="s">
+        <v>1</v>
+      </c>
+      <c r="R35" t="s">
+        <v>1</v>
+      </c>
+      <c r="S35" t="s">
+        <v>1</v>
+      </c>
+      <c r="T35" t="s">
+        <v>1</v>
+      </c>
+      <c r="U35" t="s">
+        <v>1</v>
+      </c>
+      <c r="V35" t="s">
+        <v>1</v>
+      </c>
+      <c r="W35" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>0</v>
+      </c>
+      <c r="B36" t="s">
+        <v>1</v>
+      </c>
+      <c r="C36" t="s">
+        <v>1</v>
+      </c>
+      <c r="D36" t="s">
+        <v>1</v>
+      </c>
+      <c r="E36" t="s">
+        <v>1</v>
+      </c>
+      <c r="F36" t="s">
+        <v>1</v>
+      </c>
+      <c r="G36" t="s">
+        <v>1</v>
+      </c>
+      <c r="H36" t="s">
+        <v>1</v>
+      </c>
+      <c r="I36" t="s">
+        <v>1</v>
+      </c>
+      <c r="J36" t="s">
+        <v>1</v>
+      </c>
+      <c r="K36" t="s">
+        <v>1</v>
+      </c>
+      <c r="L36" t="s">
+        <v>1</v>
+      </c>
+      <c r="M36" t="s">
+        <v>1</v>
+      </c>
+      <c r="N36" t="s">
+        <v>1</v>
+      </c>
+      <c r="O36" t="s">
+        <v>1</v>
+      </c>
+      <c r="P36" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q36" t="s">
+        <v>1</v>
+      </c>
+      <c r="R36" t="s">
+        <v>1</v>
+      </c>
+      <c r="S36" t="s">
+        <v>1</v>
+      </c>
+      <c r="T36" t="s">
+        <v>1</v>
+      </c>
+      <c r="U36" t="s">
+        <v>1</v>
+      </c>
+      <c r="V36" t="s">
+        <v>1</v>
+      </c>
+      <c r="W36" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>0</v>
+      </c>
+      <c r="B37" t="s">
+        <v>1</v>
+      </c>
+      <c r="C37" t="s">
+        <v>1</v>
+      </c>
+      <c r="D37" t="s">
+        <v>1</v>
+      </c>
+      <c r="E37" t="s">
+        <v>1</v>
+      </c>
+      <c r="F37" t="s">
+        <v>1</v>
+      </c>
+      <c r="G37" t="s">
+        <v>1</v>
+      </c>
+      <c r="H37" t="s">
+        <v>1</v>
+      </c>
+      <c r="I37" t="s">
+        <v>1</v>
+      </c>
+      <c r="J37" t="s">
+        <v>1</v>
+      </c>
+      <c r="K37" t="s">
+        <v>1</v>
+      </c>
+      <c r="L37" t="s">
+        <v>1</v>
+      </c>
+      <c r="M37" t="s">
+        <v>1</v>
+      </c>
+      <c r="N37" t="s">
+        <v>1</v>
+      </c>
+      <c r="O37" t="s">
+        <v>1</v>
+      </c>
+      <c r="P37" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q37" t="s">
+        <v>1</v>
+      </c>
+      <c r="R37" t="s">
+        <v>1</v>
+      </c>
+      <c r="S37" t="s">
+        <v>1</v>
+      </c>
+      <c r="T37" t="s">
+        <v>1</v>
+      </c>
+      <c r="U37" t="s">
+        <v>1</v>
+      </c>
+      <c r="V37" t="s">
+        <v>1</v>
+      </c>
+      <c r="W37" t="s">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
rendering fixes + start working on movement
</commit_message>
<xml_diff>
--- a/resources/map.xlsx
+++ b/resources/map.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nicol\Documents\GitHub\StoreGame\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD5E83DB-C24A-4101-A3AD-69DAAF11F1B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDE7BD23-7878-496D-BDF6-C9ED3EF5B7A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5115" yWindow="3555" windowWidth="28800" windowHeight="15885" xr2:uid="{56ED3418-DE84-4A29-B959-FE4D25080271}"/>
+    <workbookView xWindow="3600" yWindow="3090" windowWidth="28800" windowHeight="15885" xr2:uid="{56ED3418-DE84-4A29-B959-FE4D25080271}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="861" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1221" uniqueCount="6">
   <si>
     <t>WALL</t>
   </si>
@@ -44,16 +44,16 @@
     <t>GROUND</t>
   </si>
   <si>
-    <t>SHELF_N_CC:aa</t>
+    <t>SHELF_or:N_cc:aa</t>
   </si>
   <si>
-    <t>SHELF_N_CC:ab</t>
+    <t>SHELF_or:N_cc:ab</t>
   </si>
   <si>
-    <t>SHELF_S_CC:ac</t>
+    <t>SHELF_or:S_cc:ac</t>
   </si>
   <si>
-    <t>SHELF_S_CC:ad</t>
+    <t>SHELF_or:S_cc:ad</t>
   </si>
 </sst>
 </file>
@@ -427,8 +427,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{892ABF15-6683-43AF-9DBE-19CFF00B5E93}">
   <dimension ref="A1:AG37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L18" sqref="L18"/>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -604,6 +604,36 @@
       <c r="W2" t="s">
         <v>1</v>
       </c>
+      <c r="X2" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>1</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>1</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>1</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>1</v>
+      </c>
+      <c r="AC2" t="s">
+        <v>1</v>
+      </c>
+      <c r="AD2" t="s">
+        <v>1</v>
+      </c>
+      <c r="AE2" t="s">
+        <v>1</v>
+      </c>
+      <c r="AF2" t="s">
+        <v>1</v>
+      </c>
+      <c r="AG2" t="s">
+        <v>1</v>
+      </c>
     </row>
     <row r="3" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -675,6 +705,36 @@
       <c r="W3" t="s">
         <v>1</v>
       </c>
+      <c r="X3" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y3" t="s">
+        <v>1</v>
+      </c>
+      <c r="Z3" t="s">
+        <v>1</v>
+      </c>
+      <c r="AA3" t="s">
+        <v>1</v>
+      </c>
+      <c r="AB3" t="s">
+        <v>1</v>
+      </c>
+      <c r="AC3" t="s">
+        <v>1</v>
+      </c>
+      <c r="AD3" t="s">
+        <v>1</v>
+      </c>
+      <c r="AE3" t="s">
+        <v>1</v>
+      </c>
+      <c r="AF3" t="s">
+        <v>1</v>
+      </c>
+      <c r="AG3" t="s">
+        <v>1</v>
+      </c>
     </row>
     <row r="4" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -684,28 +744,28 @@
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E4" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F4" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G4" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H4" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I4" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J4" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="K4" t="s">
         <v>1</v>
@@ -744,6 +804,36 @@
         <v>1</v>
       </c>
       <c r="W4" t="s">
+        <v>1</v>
+      </c>
+      <c r="X4" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y4" t="s">
+        <v>1</v>
+      </c>
+      <c r="Z4" t="s">
+        <v>1</v>
+      </c>
+      <c r="AA4" t="s">
+        <v>1</v>
+      </c>
+      <c r="AB4" t="s">
+        <v>1</v>
+      </c>
+      <c r="AC4" t="s">
+        <v>1</v>
+      </c>
+      <c r="AD4" t="s">
+        <v>1</v>
+      </c>
+      <c r="AE4" t="s">
+        <v>1</v>
+      </c>
+      <c r="AF4" t="s">
+        <v>1</v>
+      </c>
+      <c r="AG4" t="s">
         <v>1</v>
       </c>
     </row>
@@ -755,28 +845,28 @@
         <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D5" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E5" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="F5" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="G5" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="H5" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="I5" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="J5" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="K5" t="s">
         <v>1</v>
@@ -815,6 +905,36 @@
         <v>1</v>
       </c>
       <c r="W5" t="s">
+        <v>1</v>
+      </c>
+      <c r="X5" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y5" t="s">
+        <v>1</v>
+      </c>
+      <c r="Z5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AA5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AB5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AC5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AD5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AE5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AF5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AG5" t="s">
         <v>1</v>
       </c>
     </row>
@@ -888,6 +1008,36 @@
       <c r="W6" t="s">
         <v>1</v>
       </c>
+      <c r="X6" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y6" t="s">
+        <v>1</v>
+      </c>
+      <c r="Z6" t="s">
+        <v>1</v>
+      </c>
+      <c r="AA6" t="s">
+        <v>1</v>
+      </c>
+      <c r="AB6" t="s">
+        <v>1</v>
+      </c>
+      <c r="AC6" t="s">
+        <v>1</v>
+      </c>
+      <c r="AD6" t="s">
+        <v>1</v>
+      </c>
+      <c r="AE6" t="s">
+        <v>1</v>
+      </c>
+      <c r="AF6" t="s">
+        <v>1</v>
+      </c>
+      <c r="AG6" t="s">
+        <v>1</v>
+      </c>
     </row>
     <row r="7" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
@@ -903,28 +1053,28 @@
         <v>1</v>
       </c>
       <c r="E7" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F7" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G7" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H7" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I7" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="J7" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="K7" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="L7" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="M7" t="s">
         <v>1</v>
@@ -957,6 +1107,36 @@
         <v>1</v>
       </c>
       <c r="W7" t="s">
+        <v>1</v>
+      </c>
+      <c r="X7" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y7" t="s">
+        <v>1</v>
+      </c>
+      <c r="Z7" t="s">
+        <v>1</v>
+      </c>
+      <c r="AA7" t="s">
+        <v>1</v>
+      </c>
+      <c r="AB7" t="s">
+        <v>1</v>
+      </c>
+      <c r="AC7" t="s">
+        <v>1</v>
+      </c>
+      <c r="AD7" t="s">
+        <v>1</v>
+      </c>
+      <c r="AE7" t="s">
+        <v>1</v>
+      </c>
+      <c r="AF7" t="s">
+        <v>1</v>
+      </c>
+      <c r="AG7" t="s">
         <v>1</v>
       </c>
     </row>
@@ -974,28 +1154,28 @@
         <v>1</v>
       </c>
       <c r="E8" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F8" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G8" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="H8" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="I8" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="J8" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="K8" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="L8" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="M8" t="s">
         <v>1</v>
@@ -1028,6 +1208,36 @@
         <v>1</v>
       </c>
       <c r="W8" t="s">
+        <v>1</v>
+      </c>
+      <c r="X8" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y8" t="s">
+        <v>1</v>
+      </c>
+      <c r="Z8" t="s">
+        <v>1</v>
+      </c>
+      <c r="AA8" t="s">
+        <v>1</v>
+      </c>
+      <c r="AB8" t="s">
+        <v>1</v>
+      </c>
+      <c r="AC8" t="s">
+        <v>1</v>
+      </c>
+      <c r="AD8" t="s">
+        <v>1</v>
+      </c>
+      <c r="AE8" t="s">
+        <v>1</v>
+      </c>
+      <c r="AF8" t="s">
+        <v>1</v>
+      </c>
+      <c r="AG8" t="s">
         <v>1</v>
       </c>
     </row>
@@ -1101,6 +1311,36 @@
       <c r="W9" t="s">
         <v>1</v>
       </c>
+      <c r="X9" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y9" t="s">
+        <v>1</v>
+      </c>
+      <c r="Z9" t="s">
+        <v>1</v>
+      </c>
+      <c r="AA9" t="s">
+        <v>1</v>
+      </c>
+      <c r="AB9" t="s">
+        <v>1</v>
+      </c>
+      <c r="AC9" t="s">
+        <v>1</v>
+      </c>
+      <c r="AD9" t="s">
+        <v>1</v>
+      </c>
+      <c r="AE9" t="s">
+        <v>1</v>
+      </c>
+      <c r="AF9" t="s">
+        <v>1</v>
+      </c>
+      <c r="AG9" t="s">
+        <v>1</v>
+      </c>
     </row>
     <row r="10" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
@@ -1172,6 +1412,36 @@
       <c r="W10" t="s">
         <v>1</v>
       </c>
+      <c r="X10" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y10" t="s">
+        <v>1</v>
+      </c>
+      <c r="Z10" t="s">
+        <v>1</v>
+      </c>
+      <c r="AA10" t="s">
+        <v>1</v>
+      </c>
+      <c r="AB10" t="s">
+        <v>1</v>
+      </c>
+      <c r="AC10" t="s">
+        <v>1</v>
+      </c>
+      <c r="AD10" t="s">
+        <v>1</v>
+      </c>
+      <c r="AE10" t="s">
+        <v>1</v>
+      </c>
+      <c r="AF10" t="s">
+        <v>1</v>
+      </c>
+      <c r="AG10" t="s">
+        <v>1</v>
+      </c>
     </row>
     <row r="11" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
@@ -1243,6 +1513,36 @@
       <c r="W11" t="s">
         <v>1</v>
       </c>
+      <c r="X11" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y11" t="s">
+        <v>1</v>
+      </c>
+      <c r="Z11" t="s">
+        <v>1</v>
+      </c>
+      <c r="AA11" t="s">
+        <v>1</v>
+      </c>
+      <c r="AB11" t="s">
+        <v>1</v>
+      </c>
+      <c r="AC11" t="s">
+        <v>1</v>
+      </c>
+      <c r="AD11" t="s">
+        <v>1</v>
+      </c>
+      <c r="AE11" t="s">
+        <v>1</v>
+      </c>
+      <c r="AF11" t="s">
+        <v>1</v>
+      </c>
+      <c r="AG11" t="s">
+        <v>1</v>
+      </c>
     </row>
     <row r="12" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
@@ -1314,6 +1614,36 @@
       <c r="W12" t="s">
         <v>1</v>
       </c>
+      <c r="X12" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y12" t="s">
+        <v>1</v>
+      </c>
+      <c r="Z12" t="s">
+        <v>1</v>
+      </c>
+      <c r="AA12" t="s">
+        <v>1</v>
+      </c>
+      <c r="AB12" t="s">
+        <v>1</v>
+      </c>
+      <c r="AC12" t="s">
+        <v>1</v>
+      </c>
+      <c r="AD12" t="s">
+        <v>1</v>
+      </c>
+      <c r="AE12" t="s">
+        <v>1</v>
+      </c>
+      <c r="AF12" t="s">
+        <v>1</v>
+      </c>
+      <c r="AG12" t="s">
+        <v>1</v>
+      </c>
     </row>
     <row r="13" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
@@ -1385,6 +1715,36 @@
       <c r="W13" t="s">
         <v>1</v>
       </c>
+      <c r="X13" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y13" t="s">
+        <v>1</v>
+      </c>
+      <c r="Z13" t="s">
+        <v>1</v>
+      </c>
+      <c r="AA13" t="s">
+        <v>1</v>
+      </c>
+      <c r="AB13" t="s">
+        <v>1</v>
+      </c>
+      <c r="AC13" t="s">
+        <v>1</v>
+      </c>
+      <c r="AD13" t="s">
+        <v>1</v>
+      </c>
+      <c r="AE13" t="s">
+        <v>1</v>
+      </c>
+      <c r="AF13" t="s">
+        <v>1</v>
+      </c>
+      <c r="AG13" t="s">
+        <v>1</v>
+      </c>
     </row>
     <row r="14" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
@@ -1456,6 +1816,36 @@
       <c r="W14" t="s">
         <v>1</v>
       </c>
+      <c r="X14" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y14" t="s">
+        <v>1</v>
+      </c>
+      <c r="Z14" t="s">
+        <v>1</v>
+      </c>
+      <c r="AA14" t="s">
+        <v>1</v>
+      </c>
+      <c r="AB14" t="s">
+        <v>1</v>
+      </c>
+      <c r="AC14" t="s">
+        <v>1</v>
+      </c>
+      <c r="AD14" t="s">
+        <v>1</v>
+      </c>
+      <c r="AE14" t="s">
+        <v>1</v>
+      </c>
+      <c r="AF14" t="s">
+        <v>1</v>
+      </c>
+      <c r="AG14" t="s">
+        <v>1</v>
+      </c>
     </row>
     <row r="15" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
@@ -1527,6 +1917,36 @@
       <c r="W15" t="s">
         <v>1</v>
       </c>
+      <c r="X15" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y15" t="s">
+        <v>1</v>
+      </c>
+      <c r="Z15" t="s">
+        <v>1</v>
+      </c>
+      <c r="AA15" t="s">
+        <v>1</v>
+      </c>
+      <c r="AB15" t="s">
+        <v>1</v>
+      </c>
+      <c r="AC15" t="s">
+        <v>1</v>
+      </c>
+      <c r="AD15" t="s">
+        <v>1</v>
+      </c>
+      <c r="AE15" t="s">
+        <v>1</v>
+      </c>
+      <c r="AF15" t="s">
+        <v>1</v>
+      </c>
+      <c r="AG15" t="s">
+        <v>1</v>
+      </c>
     </row>
     <row r="16" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
@@ -1598,8 +2018,38 @@
       <c r="W16" t="s">
         <v>1</v>
       </c>
+      <c r="X16" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y16" t="s">
+        <v>1</v>
+      </c>
+      <c r="Z16" t="s">
+        <v>1</v>
+      </c>
+      <c r="AA16" t="s">
+        <v>1</v>
+      </c>
+      <c r="AB16" t="s">
+        <v>1</v>
+      </c>
+      <c r="AC16" t="s">
+        <v>1</v>
+      </c>
+      <c r="AD16" t="s">
+        <v>1</v>
+      </c>
+      <c r="AE16" t="s">
+        <v>1</v>
+      </c>
+      <c r="AF16" t="s">
+        <v>1</v>
+      </c>
+      <c r="AG16" t="s">
+        <v>1</v>
+      </c>
     </row>
-    <row r="17" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>0</v>
       </c>
@@ -1669,8 +2119,38 @@
       <c r="W17" t="s">
         <v>1</v>
       </c>
+      <c r="X17" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y17" t="s">
+        <v>1</v>
+      </c>
+      <c r="Z17" t="s">
+        <v>1</v>
+      </c>
+      <c r="AA17" t="s">
+        <v>1</v>
+      </c>
+      <c r="AB17" t="s">
+        <v>1</v>
+      </c>
+      <c r="AC17" t="s">
+        <v>1</v>
+      </c>
+      <c r="AD17" t="s">
+        <v>1</v>
+      </c>
+      <c r="AE17" t="s">
+        <v>1</v>
+      </c>
+      <c r="AF17" t="s">
+        <v>1</v>
+      </c>
+      <c r="AG17" t="s">
+        <v>1</v>
+      </c>
     </row>
-    <row r="18" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>0</v>
       </c>
@@ -1740,8 +2220,38 @@
       <c r="W18" t="s">
         <v>1</v>
       </c>
+      <c r="X18" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y18" t="s">
+        <v>1</v>
+      </c>
+      <c r="Z18" t="s">
+        <v>1</v>
+      </c>
+      <c r="AA18" t="s">
+        <v>1</v>
+      </c>
+      <c r="AB18" t="s">
+        <v>1</v>
+      </c>
+      <c r="AC18" t="s">
+        <v>1</v>
+      </c>
+      <c r="AD18" t="s">
+        <v>1</v>
+      </c>
+      <c r="AE18" t="s">
+        <v>1</v>
+      </c>
+      <c r="AF18" t="s">
+        <v>1</v>
+      </c>
+      <c r="AG18" t="s">
+        <v>1</v>
+      </c>
     </row>
-    <row r="19" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>0</v>
       </c>
@@ -1811,8 +2321,38 @@
       <c r="W19" t="s">
         <v>1</v>
       </c>
+      <c r="X19" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y19" t="s">
+        <v>1</v>
+      </c>
+      <c r="Z19" t="s">
+        <v>1</v>
+      </c>
+      <c r="AA19" t="s">
+        <v>1</v>
+      </c>
+      <c r="AB19" t="s">
+        <v>1</v>
+      </c>
+      <c r="AC19" t="s">
+        <v>1</v>
+      </c>
+      <c r="AD19" t="s">
+        <v>1</v>
+      </c>
+      <c r="AE19" t="s">
+        <v>1</v>
+      </c>
+      <c r="AF19" t="s">
+        <v>1</v>
+      </c>
+      <c r="AG19" t="s">
+        <v>1</v>
+      </c>
     </row>
-    <row r="20" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>0</v>
       </c>
@@ -1882,8 +2422,38 @@
       <c r="W20" t="s">
         <v>1</v>
       </c>
+      <c r="X20" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y20" t="s">
+        <v>1</v>
+      </c>
+      <c r="Z20" t="s">
+        <v>1</v>
+      </c>
+      <c r="AA20" t="s">
+        <v>1</v>
+      </c>
+      <c r="AB20" t="s">
+        <v>1</v>
+      </c>
+      <c r="AC20" t="s">
+        <v>1</v>
+      </c>
+      <c r="AD20" t="s">
+        <v>1</v>
+      </c>
+      <c r="AE20" t="s">
+        <v>1</v>
+      </c>
+      <c r="AF20" t="s">
+        <v>1</v>
+      </c>
+      <c r="AG20" t="s">
+        <v>1</v>
+      </c>
     </row>
-    <row r="21" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>0</v>
       </c>
@@ -1953,8 +2523,38 @@
       <c r="W21" t="s">
         <v>1</v>
       </c>
+      <c r="X21" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y21" t="s">
+        <v>1</v>
+      </c>
+      <c r="Z21" t="s">
+        <v>1</v>
+      </c>
+      <c r="AA21" t="s">
+        <v>1</v>
+      </c>
+      <c r="AB21" t="s">
+        <v>1</v>
+      </c>
+      <c r="AC21" t="s">
+        <v>1</v>
+      </c>
+      <c r="AD21" t="s">
+        <v>1</v>
+      </c>
+      <c r="AE21" t="s">
+        <v>1</v>
+      </c>
+      <c r="AF21" t="s">
+        <v>1</v>
+      </c>
+      <c r="AG21" t="s">
+        <v>1</v>
+      </c>
     </row>
-    <row r="22" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>0</v>
       </c>
@@ -2024,8 +2624,38 @@
       <c r="W22" t="s">
         <v>1</v>
       </c>
+      <c r="X22" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y22" t="s">
+        <v>1</v>
+      </c>
+      <c r="Z22" t="s">
+        <v>1</v>
+      </c>
+      <c r="AA22" t="s">
+        <v>1</v>
+      </c>
+      <c r="AB22" t="s">
+        <v>1</v>
+      </c>
+      <c r="AC22" t="s">
+        <v>1</v>
+      </c>
+      <c r="AD22" t="s">
+        <v>1</v>
+      </c>
+      <c r="AE22" t="s">
+        <v>1</v>
+      </c>
+      <c r="AF22" t="s">
+        <v>1</v>
+      </c>
+      <c r="AG22" t="s">
+        <v>1</v>
+      </c>
     </row>
-    <row r="23" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>0</v>
       </c>
@@ -2095,8 +2725,38 @@
       <c r="W23" t="s">
         <v>1</v>
       </c>
+      <c r="X23" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y23" t="s">
+        <v>1</v>
+      </c>
+      <c r="Z23" t="s">
+        <v>1</v>
+      </c>
+      <c r="AA23" t="s">
+        <v>1</v>
+      </c>
+      <c r="AB23" t="s">
+        <v>1</v>
+      </c>
+      <c r="AC23" t="s">
+        <v>1</v>
+      </c>
+      <c r="AD23" t="s">
+        <v>1</v>
+      </c>
+      <c r="AE23" t="s">
+        <v>1</v>
+      </c>
+      <c r="AF23" t="s">
+        <v>1</v>
+      </c>
+      <c r="AG23" t="s">
+        <v>1</v>
+      </c>
     </row>
-    <row r="24" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>0</v>
       </c>
@@ -2166,8 +2826,38 @@
       <c r="W24" t="s">
         <v>1</v>
       </c>
+      <c r="X24" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y24" t="s">
+        <v>1</v>
+      </c>
+      <c r="Z24" t="s">
+        <v>1</v>
+      </c>
+      <c r="AA24" t="s">
+        <v>1</v>
+      </c>
+      <c r="AB24" t="s">
+        <v>1</v>
+      </c>
+      <c r="AC24" t="s">
+        <v>1</v>
+      </c>
+      <c r="AD24" t="s">
+        <v>1</v>
+      </c>
+      <c r="AE24" t="s">
+        <v>1</v>
+      </c>
+      <c r="AF24" t="s">
+        <v>1</v>
+      </c>
+      <c r="AG24" t="s">
+        <v>1</v>
+      </c>
     </row>
-    <row r="25" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>0</v>
       </c>
@@ -2237,8 +2927,38 @@
       <c r="W25" t="s">
         <v>1</v>
       </c>
+      <c r="X25" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y25" t="s">
+        <v>1</v>
+      </c>
+      <c r="Z25" t="s">
+        <v>1</v>
+      </c>
+      <c r="AA25" t="s">
+        <v>1</v>
+      </c>
+      <c r="AB25" t="s">
+        <v>1</v>
+      </c>
+      <c r="AC25" t="s">
+        <v>1</v>
+      </c>
+      <c r="AD25" t="s">
+        <v>1</v>
+      </c>
+      <c r="AE25" t="s">
+        <v>1</v>
+      </c>
+      <c r="AF25" t="s">
+        <v>1</v>
+      </c>
+      <c r="AG25" t="s">
+        <v>1</v>
+      </c>
     </row>
-    <row r="26" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>0</v>
       </c>
@@ -2308,8 +3028,38 @@
       <c r="W26" t="s">
         <v>1</v>
       </c>
+      <c r="X26" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y26" t="s">
+        <v>1</v>
+      </c>
+      <c r="Z26" t="s">
+        <v>1</v>
+      </c>
+      <c r="AA26" t="s">
+        <v>1</v>
+      </c>
+      <c r="AB26" t="s">
+        <v>1</v>
+      </c>
+      <c r="AC26" t="s">
+        <v>1</v>
+      </c>
+      <c r="AD26" t="s">
+        <v>1</v>
+      </c>
+      <c r="AE26" t="s">
+        <v>1</v>
+      </c>
+      <c r="AF26" t="s">
+        <v>1</v>
+      </c>
+      <c r="AG26" t="s">
+        <v>1</v>
+      </c>
     </row>
-    <row r="27" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>0</v>
       </c>
@@ -2379,8 +3129,38 @@
       <c r="W27" t="s">
         <v>1</v>
       </c>
+      <c r="X27" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y27" t="s">
+        <v>1</v>
+      </c>
+      <c r="Z27" t="s">
+        <v>1</v>
+      </c>
+      <c r="AA27" t="s">
+        <v>1</v>
+      </c>
+      <c r="AB27" t="s">
+        <v>1</v>
+      </c>
+      <c r="AC27" t="s">
+        <v>1</v>
+      </c>
+      <c r="AD27" t="s">
+        <v>1</v>
+      </c>
+      <c r="AE27" t="s">
+        <v>1</v>
+      </c>
+      <c r="AF27" t="s">
+        <v>1</v>
+      </c>
+      <c r="AG27" t="s">
+        <v>1</v>
+      </c>
     </row>
-    <row r="28" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>0</v>
       </c>
@@ -2450,8 +3230,38 @@
       <c r="W28" t="s">
         <v>1</v>
       </c>
+      <c r="X28" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y28" t="s">
+        <v>1</v>
+      </c>
+      <c r="Z28" t="s">
+        <v>1</v>
+      </c>
+      <c r="AA28" t="s">
+        <v>1</v>
+      </c>
+      <c r="AB28" t="s">
+        <v>1</v>
+      </c>
+      <c r="AC28" t="s">
+        <v>1</v>
+      </c>
+      <c r="AD28" t="s">
+        <v>1</v>
+      </c>
+      <c r="AE28" t="s">
+        <v>1</v>
+      </c>
+      <c r="AF28" t="s">
+        <v>1</v>
+      </c>
+      <c r="AG28" t="s">
+        <v>1</v>
+      </c>
     </row>
-    <row r="29" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>0</v>
       </c>
@@ -2521,8 +3331,38 @@
       <c r="W29" t="s">
         <v>1</v>
       </c>
+      <c r="X29" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y29" t="s">
+        <v>1</v>
+      </c>
+      <c r="Z29" t="s">
+        <v>1</v>
+      </c>
+      <c r="AA29" t="s">
+        <v>1</v>
+      </c>
+      <c r="AB29" t="s">
+        <v>1</v>
+      </c>
+      <c r="AC29" t="s">
+        <v>1</v>
+      </c>
+      <c r="AD29" t="s">
+        <v>1</v>
+      </c>
+      <c r="AE29" t="s">
+        <v>1</v>
+      </c>
+      <c r="AF29" t="s">
+        <v>1</v>
+      </c>
+      <c r="AG29" t="s">
+        <v>1</v>
+      </c>
     </row>
-    <row r="30" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>0</v>
       </c>
@@ -2592,8 +3432,38 @@
       <c r="W30" t="s">
         <v>1</v>
       </c>
+      <c r="X30" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y30" t="s">
+        <v>1</v>
+      </c>
+      <c r="Z30" t="s">
+        <v>1</v>
+      </c>
+      <c r="AA30" t="s">
+        <v>1</v>
+      </c>
+      <c r="AB30" t="s">
+        <v>1</v>
+      </c>
+      <c r="AC30" t="s">
+        <v>1</v>
+      </c>
+      <c r="AD30" t="s">
+        <v>1</v>
+      </c>
+      <c r="AE30" t="s">
+        <v>1</v>
+      </c>
+      <c r="AF30" t="s">
+        <v>1</v>
+      </c>
+      <c r="AG30" t="s">
+        <v>1</v>
+      </c>
     </row>
-    <row r="31" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>0</v>
       </c>
@@ -2663,8 +3533,38 @@
       <c r="W31" t="s">
         <v>1</v>
       </c>
+      <c r="X31" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y31" t="s">
+        <v>1</v>
+      </c>
+      <c r="Z31" t="s">
+        <v>1</v>
+      </c>
+      <c r="AA31" t="s">
+        <v>1</v>
+      </c>
+      <c r="AB31" t="s">
+        <v>1</v>
+      </c>
+      <c r="AC31" t="s">
+        <v>1</v>
+      </c>
+      <c r="AD31" t="s">
+        <v>1</v>
+      </c>
+      <c r="AE31" t="s">
+        <v>1</v>
+      </c>
+      <c r="AF31" t="s">
+        <v>1</v>
+      </c>
+      <c r="AG31" t="s">
+        <v>1</v>
+      </c>
     </row>
-    <row r="32" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>0</v>
       </c>
@@ -2734,8 +3634,38 @@
       <c r="W32" t="s">
         <v>1</v>
       </c>
+      <c r="X32" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y32" t="s">
+        <v>1</v>
+      </c>
+      <c r="Z32" t="s">
+        <v>1</v>
+      </c>
+      <c r="AA32" t="s">
+        <v>1</v>
+      </c>
+      <c r="AB32" t="s">
+        <v>1</v>
+      </c>
+      <c r="AC32" t="s">
+        <v>1</v>
+      </c>
+      <c r="AD32" t="s">
+        <v>1</v>
+      </c>
+      <c r="AE32" t="s">
+        <v>1</v>
+      </c>
+      <c r="AF32" t="s">
+        <v>1</v>
+      </c>
+      <c r="AG32" t="s">
+        <v>1</v>
+      </c>
     </row>
-    <row r="33" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>0</v>
       </c>
@@ -2805,8 +3735,38 @@
       <c r="W33" t="s">
         <v>1</v>
       </c>
+      <c r="X33" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y33" t="s">
+        <v>1</v>
+      </c>
+      <c r="Z33" t="s">
+        <v>1</v>
+      </c>
+      <c r="AA33" t="s">
+        <v>1</v>
+      </c>
+      <c r="AB33" t="s">
+        <v>1</v>
+      </c>
+      <c r="AC33" t="s">
+        <v>1</v>
+      </c>
+      <c r="AD33" t="s">
+        <v>1</v>
+      </c>
+      <c r="AE33" t="s">
+        <v>1</v>
+      </c>
+      <c r="AF33" t="s">
+        <v>1</v>
+      </c>
+      <c r="AG33" t="s">
+        <v>1</v>
+      </c>
     </row>
-    <row r="34" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>0</v>
       </c>
@@ -2876,8 +3836,38 @@
       <c r="W34" t="s">
         <v>1</v>
       </c>
+      <c r="X34" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y34" t="s">
+        <v>1</v>
+      </c>
+      <c r="Z34" t="s">
+        <v>1</v>
+      </c>
+      <c r="AA34" t="s">
+        <v>1</v>
+      </c>
+      <c r="AB34" t="s">
+        <v>1</v>
+      </c>
+      <c r="AC34" t="s">
+        <v>1</v>
+      </c>
+      <c r="AD34" t="s">
+        <v>1</v>
+      </c>
+      <c r="AE34" t="s">
+        <v>1</v>
+      </c>
+      <c r="AF34" t="s">
+        <v>1</v>
+      </c>
+      <c r="AG34" t="s">
+        <v>1</v>
+      </c>
     </row>
-    <row r="35" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>0</v>
       </c>
@@ -2947,8 +3937,38 @@
       <c r="W35" t="s">
         <v>1</v>
       </c>
+      <c r="X35" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y35" t="s">
+        <v>1</v>
+      </c>
+      <c r="Z35" t="s">
+        <v>1</v>
+      </c>
+      <c r="AA35" t="s">
+        <v>1</v>
+      </c>
+      <c r="AB35" t="s">
+        <v>1</v>
+      </c>
+      <c r="AC35" t="s">
+        <v>1</v>
+      </c>
+      <c r="AD35" t="s">
+        <v>1</v>
+      </c>
+      <c r="AE35" t="s">
+        <v>1</v>
+      </c>
+      <c r="AF35" t="s">
+        <v>1</v>
+      </c>
+      <c r="AG35" t="s">
+        <v>1</v>
+      </c>
     </row>
-    <row r="36" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>0</v>
       </c>
@@ -3018,8 +4038,38 @@
       <c r="W36" t="s">
         <v>1</v>
       </c>
+      <c r="X36" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y36" t="s">
+        <v>1</v>
+      </c>
+      <c r="Z36" t="s">
+        <v>1</v>
+      </c>
+      <c r="AA36" t="s">
+        <v>1</v>
+      </c>
+      <c r="AB36" t="s">
+        <v>1</v>
+      </c>
+      <c r="AC36" t="s">
+        <v>1</v>
+      </c>
+      <c r="AD36" t="s">
+        <v>1</v>
+      </c>
+      <c r="AE36" t="s">
+        <v>1</v>
+      </c>
+      <c r="AF36" t="s">
+        <v>1</v>
+      </c>
+      <c r="AG36" t="s">
+        <v>1</v>
+      </c>
     </row>
-    <row r="37" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>0</v>
       </c>
@@ -3087,6 +4137,36 @@
         <v>1</v>
       </c>
       <c r="W37" t="s">
+        <v>1</v>
+      </c>
+      <c r="X37" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y37" t="s">
+        <v>1</v>
+      </c>
+      <c r="Z37" t="s">
+        <v>1</v>
+      </c>
+      <c r="AA37" t="s">
+        <v>1</v>
+      </c>
+      <c r="AB37" t="s">
+        <v>1</v>
+      </c>
+      <c r="AC37" t="s">
+        <v>1</v>
+      </c>
+      <c r="AD37" t="s">
+        <v>1</v>
+      </c>
+      <c r="AE37" t="s">
+        <v>1</v>
+      </c>
+      <c r="AF37" t="s">
+        <v>1</v>
+      </c>
+      <c r="AG37" t="s">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fixing render issues & clean up camera & start hover logic
</commit_message>
<xml_diff>
--- a/resources/map.xlsx
+++ b/resources/map.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nicol\Documents\GitHub\StoreGame\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE972068-0B93-432C-9BC5-40E19BC33EAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FB8088E-50B4-4E86-98DB-2897F824CA9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2670" yWindow="1260" windowWidth="28800" windowHeight="15885" xr2:uid="{56ED3418-DE84-4A29-B959-FE4D25080271}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21840" xr2:uid="{56ED3418-DE84-4A29-B959-FE4D25080271}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -428,7 +428,7 @@
   <dimension ref="A1:AY61"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="AS41" sqref="AS41"/>
+      <selection activeCell="AJ7" sqref="AJ7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1440,28 +1440,28 @@
         <v>1</v>
       </c>
       <c r="Z7" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AA7" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AB7" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AC7" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AD7" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="AE7" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="AF7" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="AG7" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="AH7" t="s">
         <v>1</v>
@@ -1595,28 +1595,28 @@
         <v>1</v>
       </c>
       <c r="Z8" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="AA8" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="AB8" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="AC8" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="AD8" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="AE8" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="AF8" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="AG8" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="AH8" t="s">
         <v>1</v>

</xml_diff>